<commit_message>
Update new version 2.2
</commit_message>
<xml_diff>
--- a/assets/models_history.xlsx
+++ b/assets/models_history.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\libs\mealpy\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\libs\mealpy\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1275" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1287" uniqueCount="232">
   <si>
     <t>Group</t>
   </si>
@@ -698,6 +698,24 @@
   </si>
   <si>
     <t>Dummy</t>
+  </si>
+  <si>
+    <t>Gradient-Based Optimizer</t>
+  </si>
+  <si>
+    <t>GBO</t>
+  </si>
+  <si>
+    <t>Chaos Game Optimization</t>
+  </si>
+  <si>
+    <t>CGO</t>
+  </si>
+  <si>
+    <t>FFA</t>
+  </si>
+  <si>
+    <t>Nake Mole-Rat Algorithm</t>
   </si>
 </sst>
 </file>
@@ -1238,7 +1256,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1263,9 +1281,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -4897,15 +4912,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I100"/>
+  <dimension ref="A1:I102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="C96" sqref="A1:I100"/>
+    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
+      <selection activeCell="F100" sqref="A1:I102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="13.21875" style="15" customWidth="1"/>
+    <col min="1" max="1" width="13.21875" style="14" customWidth="1"/>
     <col min="2" max="2" width="8.88671875" style="8"/>
     <col min="3" max="3" width="43.109375" style="8" customWidth="1"/>
     <col min="4" max="4" width="10" style="8" customWidth="1"/>
@@ -4918,2760 +4933,2818 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.6">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="13" t="s">
         <v>215</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="13" t="s">
         <v>218</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="I1" s="13" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15.6" customHeight="1">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="12" t="s">
         <v>165</v>
       </c>
-      <c r="B2" s="9">
+      <c r="B2" s="12">
         <v>1</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="9">
+      <c r="E2" s="12">
         <v>1964</v>
       </c>
-      <c r="F2" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="9" t="s">
+      <c r="F2" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="12" t="s">
         <v>219</v>
       </c>
-      <c r="H2" s="9">
+      <c r="H2" s="12">
         <v>3</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="I2" s="12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="15.6">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="12" t="s">
         <v>165</v>
       </c>
-      <c r="B3" s="9">
+      <c r="B3" s="12">
         <v>2</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="9">
+      <c r="E3" s="12">
         <v>1971</v>
       </c>
-      <c r="F3" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" s="9" t="s">
+      <c r="F3" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="12" t="s">
         <v>219</v>
       </c>
-      <c r="H3" s="9">
+      <c r="H3" s="12">
         <v>3</v>
       </c>
-      <c r="I3" s="9" t="s">
+      <c r="I3" s="12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.6">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="12" t="s">
         <v>165</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4" s="12">
         <v>3</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4" s="12">
         <v>1989</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="12" t="s">
         <v>216</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="G4" s="12" t="s">
         <v>219</v>
       </c>
-      <c r="H4" s="9">
+      <c r="H4" s="12">
         <v>7</v>
       </c>
-      <c r="I4" s="9" t="s">
+      <c r="I4" s="12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="15.6">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="12" t="s">
         <v>165</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B5" s="12">
         <v>3</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5" s="12">
         <v>1992</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="F5" s="12" t="s">
         <v>217</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="G5" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="H5" s="9">
+      <c r="H5" s="12">
         <v>4</v>
       </c>
-      <c r="I5" s="9" t="s">
+      <c r="I5" s="12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="15.6">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="12" t="s">
         <v>165</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6" s="12">
         <v>4</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="12">
         <v>1997</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="F6" s="12" t="s">
         <v>217</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="G6" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="H6" s="9">
+      <c r="H6" s="12">
         <v>4</v>
       </c>
-      <c r="I6" s="9" t="s">
+      <c r="I6" s="12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="15.6">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="12" t="s">
         <v>165</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B7" s="12">
         <v>5</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="9">
+      <c r="E7" s="12">
         <v>2014</v>
       </c>
-      <c r="F7" s="9" t="s">
+      <c r="F7" s="12" t="s">
         <v>217</v>
       </c>
-      <c r="G7" s="9" t="s">
+      <c r="G7" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="H7" s="9">
+      <c r="H7" s="12">
         <v>3</v>
       </c>
-      <c r="I7" s="9" t="s">
+      <c r="I7" s="12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="15.6">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="12" t="s">
         <v>165</v>
       </c>
-      <c r="B8" s="9">
+      <c r="B8" s="12">
         <v>6</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="9">
+      <c r="E8" s="12">
         <v>2014</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="F8" s="12" t="s">
         <v>217</v>
       </c>
-      <c r="G8" s="9" t="s">
+      <c r="G8" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="H8" s="9">
+      <c r="H8" s="12">
         <v>7</v>
       </c>
-      <c r="I8" s="9" t="s">
+      <c r="I8" s="12" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="15.6">
-      <c r="A9" s="13">
+      <c r="A9" s="12">
         <v>0</v>
       </c>
-      <c r="B9" s="13">
+      <c r="B9" s="12">
         <v>7</v>
       </c>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
     </row>
     <row r="10" spans="1:9" ht="15.6">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="9">
+      <c r="B10" s="12">
         <v>1</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D10" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="E10" s="9">
+      <c r="E10" s="12">
         <v>1995</v>
       </c>
-      <c r="F10" s="9" t="s">
+      <c r="F10" s="12" t="s">
         <v>217</v>
       </c>
-      <c r="G10" s="9" t="s">
+      <c r="G10" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="H10" s="9">
+      <c r="H10" s="12">
         <v>6</v>
       </c>
-      <c r="I10" s="9" t="s">
+      <c r="I10" s="12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="15.6">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="9">
+      <c r="B11" s="12">
         <v>2</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="E11" s="9">
+      <c r="E11" s="12">
         <v>2002</v>
       </c>
-      <c r="F11" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="G11" s="9" t="s">
+      <c r="F11" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="H11" s="9">
+      <c r="H11" s="12">
         <v>9</v>
       </c>
-      <c r="I11" s="9" t="s">
+      <c r="I11" s="12" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="15.6">
-      <c r="A12" s="13" t="s">
+      <c r="A12" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="9">
+      <c r="B12" s="12">
         <v>3</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C12" s="9" t="s">
         <v>199</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D12" s="12" t="s">
         <v>200</v>
       </c>
-      <c r="E12" s="9">
+      <c r="E12" s="12">
         <v>2005</v>
       </c>
-      <c r="F12" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="G12" s="9" t="s">
+      <c r="F12" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G12" s="12" t="s">
         <v>219</v>
       </c>
-      <c r="H12" s="9">
+      <c r="H12" s="12">
         <v>9</v>
       </c>
-      <c r="I12" s="9" t="s">
+      <c r="I12" s="12" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="15.6">
-      <c r="A13" s="13" t="s">
+      <c r="A13" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="9">
+      <c r="B13" s="12">
         <v>4</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="D13" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="E13" s="9">
+      <c r="E13" s="12">
         <v>2006</v>
       </c>
-      <c r="F13" s="9" t="s">
+      <c r="F13" s="12" t="s">
         <v>216</v>
       </c>
-      <c r="G13" s="9" t="s">
+      <c r="G13" s="12" t="s">
         <v>219</v>
       </c>
-      <c r="H13" s="9">
+      <c r="H13" s="12">
         <v>9</v>
       </c>
-      <c r="I13" s="9" t="s">
+      <c r="I13" s="12" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="15.6">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="9">
+      <c r="B14" s="12">
         <v>5</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="12" t="s">
         <v>181</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="D14" s="12" t="s">
         <v>182</v>
       </c>
-      <c r="E14" s="9">
+      <c r="E14" s="12">
         <v>2006</v>
       </c>
-      <c r="F14" s="9" t="s">
+      <c r="F14" s="12" t="s">
         <v>217</v>
       </c>
-      <c r="G14" s="9" t="s">
+      <c r="G14" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="H14" s="9">
+      <c r="H14" s="12">
         <v>5</v>
       </c>
-      <c r="I14" s="9" t="s">
+      <c r="I14" s="12" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="15.6">
-      <c r="A15" s="13" t="s">
+      <c r="A15" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="9">
+      <c r="B15" s="12">
         <v>6</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="D15" s="9" t="s">
+      <c r="D15" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="E15" s="9">
+      <c r="E15" s="12">
         <v>2007</v>
       </c>
-      <c r="F15" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="G15" s="9" t="s">
+      <c r="F15" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="H15" s="9">
+      <c r="H15" s="12">
         <v>8</v>
       </c>
-      <c r="I15" s="9" t="s">
+      <c r="I15" s="12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="15.6">
-      <c r="A16" s="13" t="s">
+      <c r="A16" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="9">
+      <c r="B16" s="12">
         <v>7</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="C16" s="9" t="s">
         <v>181</v>
       </c>
-      <c r="D16" s="9" t="s">
+      <c r="D16" s="12" t="s">
         <v>201</v>
       </c>
-      <c r="E16" s="9">
+      <c r="E16" s="12">
         <v>2008</v>
       </c>
-      <c r="F16" s="9" t="s">
+      <c r="F16" s="12" t="s">
         <v>217</v>
       </c>
-      <c r="G16" s="9" t="s">
+      <c r="G16" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="H16" s="9">
+      <c r="H16" s="12">
         <v>5</v>
       </c>
-      <c r="I16" s="9" t="s">
+      <c r="I16" s="12" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="15.6">
-      <c r="A17" s="13" t="s">
+      <c r="A17" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="9">
+      <c r="B17" s="12">
         <v>8</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="C17" s="9" t="s">
         <v>205</v>
       </c>
-      <c r="D17" s="9" t="s">
+      <c r="D17" s="12" t="s">
         <v>206</v>
       </c>
-      <c r="E17" s="9">
+      <c r="E17" s="12">
         <v>2009</v>
       </c>
-      <c r="F17" s="9" t="s">
+      <c r="F17" s="12" t="s">
         <v>217</v>
       </c>
-      <c r="G17" s="9" t="s">
+      <c r="G17" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="H17" s="9">
+      <c r="H17" s="12">
         <v>3</v>
       </c>
-      <c r="I17" s="9" t="s">
+      <c r="I17" s="12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="15.6">
-      <c r="A18" s="13" t="s">
+      <c r="A18" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B18" s="9">
+      <c r="B18" s="12">
         <v>9</v>
       </c>
-      <c r="C18" s="10" t="s">
+      <c r="C18" s="9" t="s">
         <v>197</v>
       </c>
-      <c r="D18" s="9" t="s">
-        <v>198</v>
-      </c>
-      <c r="E18" s="9">
+      <c r="D18" s="12" t="s">
+        <v>230</v>
+      </c>
+      <c r="E18" s="12">
         <v>2009</v>
       </c>
-      <c r="F18" s="9" t="s">
+      <c r="F18" s="12" t="s">
         <v>216</v>
       </c>
-      <c r="G18" s="9" t="s">
+      <c r="G18" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="H18" s="9">
+      <c r="H18" s="12">
         <v>8</v>
       </c>
-      <c r="I18" s="9" t="s">
+      <c r="I18" s="12" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="15.6">
-      <c r="A19" s="13" t="s">
+      <c r="A19" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B19" s="9">
+      <c r="B19" s="12">
         <v>10</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="C19" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="D19" s="9" t="s">
+      <c r="D19" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="E19" s="9">
+      <c r="E19" s="12">
         <v>2010</v>
       </c>
-      <c r="F19" s="9" t="s">
+      <c r="F19" s="12" t="s">
         <v>216</v>
       </c>
-      <c r="G19" s="9" t="s">
+      <c r="G19" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="H19" s="9">
+      <c r="H19" s="12">
         <v>7</v>
       </c>
-      <c r="I19" s="9" t="s">
+      <c r="I19" s="12" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="15.6">
-      <c r="A20" s="13" t="s">
+      <c r="A20" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B20" s="9">
+      <c r="B20" s="12">
         <v>11</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="D20" s="9" t="s">
+      <c r="D20" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="E20" s="9">
+      <c r="E20" s="12">
         <v>2010</v>
       </c>
-      <c r="F20" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="G20" s="9" t="s">
+      <c r="F20" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G20" s="12" t="s">
         <v>219</v>
       </c>
-      <c r="H20" s="9">
+      <c r="H20" s="12">
         <v>5</v>
       </c>
-      <c r="I20" s="9" t="s">
+      <c r="I20" s="12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="15.6">
-      <c r="A21" s="13" t="s">
+      <c r="A21" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B21" s="9">
+      <c r="B21" s="12">
         <v>12</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="C21" s="12" t="s">
         <v>174</v>
       </c>
-      <c r="D21" s="9" t="s">
+      <c r="D21" s="12" t="s">
         <v>175</v>
       </c>
-      <c r="E21" s="9">
+      <c r="E21" s="12">
         <v>2012</v>
       </c>
-      <c r="F21" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="G21" s="9" t="s">
+      <c r="F21" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G21" s="12" t="s">
         <v>219</v>
       </c>
-      <c r="H21" s="9">
+      <c r="H21" s="12">
         <v>2</v>
       </c>
-      <c r="I21" s="9" t="s">
+      <c r="I21" s="12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="15.6">
-      <c r="A22" s="13" t="s">
+      <c r="A22" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B22" s="9">
-        <v>13</v>
-      </c>
-      <c r="C22" s="9" t="s">
+      <c r="B22" s="12">
+        <v>13</v>
+      </c>
+      <c r="C22" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="D22" s="9" t="s">
+      <c r="D22" s="12" t="s">
         <v>213</v>
       </c>
-      <c r="E22" s="9">
+      <c r="E22" s="12">
         <v>2013</v>
       </c>
-      <c r="F22" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="G22" s="9" t="s">
+      <c r="F22" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G22" s="12" t="s">
         <v>219</v>
       </c>
-      <c r="H22" s="9">
+      <c r="H22" s="12">
         <v>3</v>
       </c>
-      <c r="I22" s="9" t="s">
+      <c r="I22" s="12" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="15.6">
-      <c r="A23" s="13" t="s">
+      <c r="A23" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B23" s="9">
+      <c r="B23" s="12">
         <v>14</v>
       </c>
-      <c r="C23" s="9" t="s">
+      <c r="C23" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="D23" s="9" t="s">
+      <c r="D23" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="E23" s="9">
+      <c r="E23" s="12">
         <v>2014</v>
       </c>
-      <c r="F23" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="G23" s="9" t="s">
+      <c r="F23" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G23" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="H23" s="9">
+      <c r="H23" s="12">
         <v>2</v>
       </c>
-      <c r="I23" s="9" t="s">
+      <c r="I23" s="12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="15.6">
-      <c r="A24" s="13" t="s">
+      <c r="A24" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B24" s="9">
-        <v>15</v>
-      </c>
-      <c r="C24" s="9" t="s">
+      <c r="B24" s="12">
+        <v>15</v>
+      </c>
+      <c r="C24" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="D24" s="9" t="s">
+      <c r="D24" s="12" t="s">
         <v>214</v>
       </c>
-      <c r="E24" s="9">
+      <c r="E24" s="12">
         <v>2015</v>
       </c>
-      <c r="F24" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="G24" s="9" t="s">
+      <c r="F24" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G24" s="12" t="s">
         <v>219</v>
       </c>
-      <c r="H24" s="9">
+      <c r="H24" s="12">
         <v>5</v>
       </c>
-      <c r="I24" s="9" t="s">
+      <c r="I24" s="12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="15.6">
-      <c r="A25" s="13" t="s">
+      <c r="A25" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B25" s="9">
+      <c r="B25" s="12">
         <v>16</v>
       </c>
-      <c r="C25" s="9" t="s">
+      <c r="C25" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="D25" s="9" t="s">
+      <c r="D25" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="E25" s="9">
+      <c r="E25" s="12">
         <v>2015</v>
       </c>
-      <c r="F25" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="G25" s="9" t="s">
+      <c r="F25" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G25" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="H25" s="9">
+      <c r="H25" s="12">
         <v>2</v>
       </c>
-      <c r="I25" s="9" t="s">
+      <c r="I25" s="12" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="15.6">
-      <c r="A26" s="13" t="s">
+      <c r="A26" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B26" s="9">
+      <c r="B26" s="12">
         <v>17</v>
       </c>
-      <c r="C26" s="9" t="s">
+      <c r="C26" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="D26" s="9" t="s">
+      <c r="D26" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="E26" s="9">
+      <c r="E26" s="12">
         <v>2015</v>
       </c>
-      <c r="F26" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="G26" s="9" t="s">
+      <c r="F26" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G26" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="H26" s="9">
+      <c r="H26" s="12">
         <v>2</v>
       </c>
-      <c r="I26" s="9" t="s">
+      <c r="I26" s="12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="15.6">
-      <c r="A27" s="13" t="s">
+      <c r="A27" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B27" s="9">
+      <c r="B27" s="12">
         <v>18</v>
       </c>
-      <c r="C27" s="9" t="s">
+      <c r="C27" s="12" t="s">
         <v>169</v>
       </c>
-      <c r="D27" s="9" t="s">
+      <c r="D27" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="E27" s="9">
+      <c r="E27" s="12">
         <v>2015</v>
       </c>
-      <c r="F27" s="9" t="s">
+      <c r="F27" s="12" t="s">
         <v>216</v>
       </c>
-      <c r="G27" s="9" t="s">
+      <c r="G27" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="H27" s="9">
+      <c r="H27" s="12">
         <v>5</v>
       </c>
-      <c r="I27" s="9" t="s">
+      <c r="I27" s="12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="15.6">
-      <c r="A28" s="13" t="s">
+      <c r="A28" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B28" s="9">
+      <c r="B28" s="12">
         <v>19</v>
       </c>
-      <c r="C28" s="10" t="s">
+      <c r="C28" s="9" t="s">
         <v>176</v>
       </c>
-      <c r="D28" s="9" t="s">
+      <c r="D28" s="12" t="s">
         <v>177</v>
       </c>
-      <c r="E28" s="9">
+      <c r="E28" s="12">
         <v>2016</v>
       </c>
-      <c r="F28" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="G28" s="9" t="s">
+      <c r="F28" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G28" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="H28" s="9">
+      <c r="H28" s="12">
         <v>2</v>
       </c>
-      <c r="I28" s="9" t="s">
+      <c r="I28" s="12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="15.6">
-      <c r="A29" s="13" t="s">
+      <c r="A29" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B29" s="9">
+      <c r="B29" s="12">
         <v>20</v>
       </c>
-      <c r="C29" s="9" t="s">
+      <c r="C29" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="D29" s="9" t="s">
+      <c r="D29" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="E29" s="9">
+      <c r="E29" s="12">
         <v>2016</v>
       </c>
-      <c r="F29" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="G29" s="9" t="s">
+      <c r="F29" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G29" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="H29" s="9">
+      <c r="H29" s="12">
         <v>2</v>
       </c>
-      <c r="I29" s="9" t="s">
+      <c r="I29" s="12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="15.6">
-      <c r="A30" s="13" t="s">
+      <c r="A30" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B30" s="9">
+      <c r="B30" s="12">
         <v>21</v>
       </c>
-      <c r="C30" s="10" t="s">
+      <c r="C30" s="9" t="s">
         <v>195</v>
       </c>
-      <c r="D30" s="9" t="s">
+      <c r="D30" s="12" t="s">
         <v>196</v>
       </c>
-      <c r="E30" s="9">
+      <c r="E30" s="12">
         <v>2016</v>
       </c>
-      <c r="F30" s="9" t="s">
+      <c r="F30" s="12" t="s">
         <v>216</v>
       </c>
-      <c r="G30" s="9" t="s">
+      <c r="G30" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="H30" s="9">
+      <c r="H30" s="12">
         <v>2</v>
       </c>
-      <c r="I30" s="9" t="s">
+      <c r="I30" s="12" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="15.6">
-      <c r="A31" s="13" t="s">
+      <c r="A31" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B31" s="9">
+      <c r="B31" s="12">
         <v>22</v>
       </c>
-      <c r="C31" s="9" t="s">
+      <c r="C31" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="D31" s="9" t="s">
+      <c r="D31" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="E31" s="9">
+      <c r="E31" s="12">
         <v>2016</v>
       </c>
-      <c r="F31" s="9" t="s">
+      <c r="F31" s="12" t="s">
         <v>217</v>
       </c>
-      <c r="G31" s="9" t="s">
+      <c r="G31" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="H31" s="9">
+      <c r="H31" s="12">
         <v>9</v>
       </c>
-      <c r="I31" s="9" t="s">
+      <c r="I31" s="12" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="15.6">
-      <c r="A32" s="13" t="s">
+      <c r="A32" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B32" s="9">
+      <c r="B32" s="12">
         <v>23</v>
       </c>
-      <c r="C32" s="11" t="s">
+      <c r="C32" s="10" t="s">
         <v>170</v>
       </c>
-      <c r="D32" s="9" t="s">
+      <c r="D32" s="12" t="s">
         <v>171</v>
       </c>
-      <c r="E32" s="9">
+      <c r="E32" s="12">
         <v>2017</v>
       </c>
-      <c r="F32" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="G32" s="9" t="s">
+      <c r="F32" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G32" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="H32" s="9">
+      <c r="H32" s="12">
         <v>6</v>
       </c>
-      <c r="I32" s="9" t="s">
+      <c r="I32" s="12" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="15.6">
-      <c r="A33" s="13" t="s">
+      <c r="A33" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B33" s="9">
+      <c r="B33" s="12">
         <v>24</v>
       </c>
-      <c r="C33" s="10" t="s">
+      <c r="C33" s="9" t="s">
         <v>193</v>
       </c>
-      <c r="D33" s="9" t="s">
+      <c r="D33" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="E33" s="9">
+      <c r="E33" s="12">
         <v>2017</v>
       </c>
-      <c r="F33" s="9" t="s">
+      <c r="F33" s="12" t="s">
         <v>216</v>
       </c>
-      <c r="G33" s="9" t="s">
+      <c r="G33" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="H33" s="9">
+      <c r="H33" s="12">
         <v>2</v>
       </c>
-      <c r="I33" s="9" t="s">
+      <c r="I33" s="12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="15.6">
-      <c r="A34" s="13" t="s">
+      <c r="A34" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B34" s="9">
+      <c r="B34" s="12">
         <v>25</v>
       </c>
-      <c r="C34" s="9" t="s">
+      <c r="C34" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="D34" s="9" t="s">
+      <c r="D34" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="E34" s="9">
+      <c r="E34" s="12">
         <v>2017</v>
       </c>
-      <c r="F34" s="9" t="s">
+      <c r="F34" s="12" t="s">
         <v>217</v>
       </c>
-      <c r="G34" s="9" t="s">
+      <c r="G34" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="H34" s="9">
+      <c r="H34" s="12">
         <v>2</v>
       </c>
-      <c r="I34" s="9" t="s">
+      <c r="I34" s="12" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="15.6">
-      <c r="A35" s="13" t="s">
+      <c r="A35" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B35" s="9">
+      <c r="B35" s="12">
         <v>26</v>
       </c>
-      <c r="C35" s="9" t="s">
+      <c r="C35" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="D35" s="9" t="s">
+      <c r="D35" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="E35" s="9">
+      <c r="E35" s="12">
         <v>2017</v>
       </c>
-      <c r="F35" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="G35" s="9" t="s">
+      <c r="F35" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G35" s="12" t="s">
         <v>219</v>
       </c>
-      <c r="H35" s="9">
+      <c r="H35" s="12">
         <v>3</v>
       </c>
-      <c r="I35" s="9" t="s">
+      <c r="I35" s="12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="15.6">
-      <c r="A36" s="13" t="s">
+      <c r="A36" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B36" s="9">
+      <c r="B36" s="12">
         <v>27</v>
       </c>
-      <c r="C36" s="9" t="s">
+      <c r="C36" s="12" t="s">
         <v>223</v>
       </c>
-      <c r="D36" s="9" t="s">
+      <c r="D36" s="12" t="s">
         <v>224</v>
       </c>
-      <c r="E36" s="9">
+      <c r="E36" s="12">
         <v>2018</v>
       </c>
-      <c r="F36" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="G36" s="9" t="s">
+      <c r="F36" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G36" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="H36" s="9">
+      <c r="H36" s="12">
         <v>3</v>
       </c>
-      <c r="I36" s="9" t="s">
+      <c r="I36" s="12" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="15.6">
-      <c r="A37" s="13" t="s">
+      <c r="A37" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B37" s="9">
+      <c r="B37" s="12">
         <v>28</v>
       </c>
-      <c r="C37" s="9" t="s">
+      <c r="C37" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="D37" s="9" t="s">
+      <c r="D37" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="E37" s="9">
+      <c r="E37" s="12">
         <v>2018</v>
       </c>
-      <c r="F37" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="G37" s="9" t="s">
+      <c r="F37" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G37" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="H37" s="9">
+      <c r="H37" s="12">
         <v>5</v>
       </c>
-      <c r="I37" s="9" t="s">
+      <c r="I37" s="12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="15.6">
-      <c r="A38" s="13" t="s">
+      <c r="A38" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B38" s="9">
+      <c r="B38" s="12">
         <v>29</v>
       </c>
-      <c r="C38" s="9" t="s">
+      <c r="C38" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="D38" s="9" t="s">
+      <c r="D38" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="E38" s="9">
+      <c r="E38" s="12">
         <v>2019</v>
       </c>
-      <c r="F38" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="G38" s="9" t="s">
+      <c r="F38" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G38" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="H38" s="9">
+      <c r="H38" s="12">
         <v>2</v>
       </c>
-      <c r="I38" s="9" t="s">
+      <c r="I38" s="12" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="15.6">
-      <c r="A39" s="13" t="s">
+      <c r="A39" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B39" s="9">
+      <c r="B39" s="12">
         <v>30</v>
       </c>
-      <c r="C39" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="D39" s="9" t="s">
+      <c r="C39" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="D39" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="E39" s="9">
+      <c r="E39" s="12">
         <v>2019</v>
       </c>
-      <c r="F39" s="9" t="s">
+      <c r="F39" s="12" t="s">
         <v>217</v>
       </c>
-      <c r="G39" s="9" t="s">
+      <c r="G39" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="H39" s="9">
+      <c r="H39" s="12">
         <v>3</v>
       </c>
-      <c r="I39" s="9" t="s">
+      <c r="I39" s="12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="15.6">
-      <c r="A40" s="13" t="s">
+      <c r="A40" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B40" s="9">
+      <c r="B40" s="12">
         <v>31</v>
       </c>
-      <c r="C40" s="9" t="s">
+      <c r="C40" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="D40" s="9" t="s">
+      <c r="D40" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="E40" s="9">
+      <c r="E40" s="12">
         <v>2019</v>
       </c>
-      <c r="F40" s="9" t="s">
+      <c r="F40" s="12" t="s">
         <v>217</v>
       </c>
-      <c r="G40" s="9" t="s">
+      <c r="G40" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="H40" s="9">
+      <c r="H40" s="12">
         <v>7</v>
       </c>
-      <c r="I40" s="9" t="s">
+      <c r="I40" s="12" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="15.6">
-      <c r="A41" s="13" t="s">
+      <c r="A41" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B41" s="9">
+      <c r="B41" s="12">
         <v>32</v>
       </c>
-      <c r="C41" s="9" t="s">
+      <c r="C41" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="D41" s="9" t="s">
+      <c r="D41" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="E41" s="9">
+      <c r="E41" s="12">
         <v>2019</v>
       </c>
-      <c r="F41" s="9" t="s">
+      <c r="F41" s="12" t="s">
         <v>216</v>
       </c>
-      <c r="G41" s="9" t="s">
+      <c r="G41" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="H41" s="9">
+      <c r="H41" s="12">
         <v>2</v>
       </c>
-      <c r="I41" s="9" t="s">
+      <c r="I41" s="12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="15.6">
-      <c r="A42" s="13" t="s">
+      <c r="A42" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B42" s="9">
+      <c r="B42" s="12">
         <v>33</v>
       </c>
-      <c r="C42" s="9" t="s">
+      <c r="C42" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="D42" s="9" t="s">
+      <c r="D42" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="E42" s="9">
+      <c r="E42" s="12">
         <v>2019</v>
       </c>
-      <c r="F42" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="G42" s="9" t="s">
+      <c r="F42" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G42" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="H42" s="9">
+      <c r="H42" s="12">
         <v>5</v>
       </c>
-      <c r="I42" s="9" t="s">
+      <c r="I42" s="12" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="15.6">
-      <c r="A43" s="13" t="s">
+      <c r="A43" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B43" s="9">
+      <c r="B43" s="12">
         <v>34</v>
       </c>
-      <c r="C43" s="9" t="s">
+      <c r="C43" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="D43" s="9" t="s">
+      <c r="D43" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="E43" s="9">
+      <c r="E43" s="12">
         <v>2019</v>
       </c>
-      <c r="F43" s="9" t="s">
+      <c r="F43" s="12" t="s">
         <v>216</v>
       </c>
-      <c r="G43" s="9" t="s">
+      <c r="G43" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="H43" s="9">
+      <c r="H43" s="12">
         <v>2</v>
       </c>
-      <c r="I43" s="9" t="s">
+      <c r="I43" s="12" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="15.6">
-      <c r="A44" s="13" t="s">
+      <c r="A44" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B44" s="9">
+      <c r="B44" s="12">
         <v>35</v>
       </c>
-      <c r="C44" s="9" t="s">
+      <c r="C44" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="D44" s="9" t="s">
+      <c r="D44" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="E44" s="9">
+      <c r="E44" s="12">
         <v>2020</v>
       </c>
-      <c r="F44" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="G44" s="9" t="s">
+      <c r="F44" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G44" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="H44" s="9">
+      <c r="H44" s="12">
         <v>3</v>
       </c>
-      <c r="I44" s="9" t="s">
+      <c r="I44" s="12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="45" spans="1:9" ht="15.6">
-      <c r="A45" s="13" t="s">
+      <c r="A45" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B45" s="9">
+      <c r="B45" s="12">
         <v>36</v>
       </c>
-      <c r="C45" s="9" t="s">
+      <c r="C45" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="D45" s="9" t="s">
+      <c r="D45" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="E45" s="9">
+      <c r="E45" s="12">
         <v>2020</v>
       </c>
-      <c r="F45" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="G45" s="9" t="s">
+      <c r="F45" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G45" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="H45" s="9">
+      <c r="H45" s="12">
         <v>5</v>
       </c>
-      <c r="I45" s="9" t="s">
+      <c r="I45" s="12" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="46" spans="1:9" ht="15.6">
-      <c r="A46" s="13" t="s">
+      <c r="A46" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B46" s="9">
+      <c r="B46" s="12">
         <v>37</v>
       </c>
-      <c r="C46" s="9" t="s">
+      <c r="C46" s="12" t="s">
         <v>203</v>
       </c>
-      <c r="D46" s="9" t="s">
+      <c r="D46" s="12" t="s">
         <v>204</v>
       </c>
-      <c r="E46" s="9">
+      <c r="E46" s="12">
         <v>2021</v>
       </c>
-      <c r="F46" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="G46" s="9" t="s">
+      <c r="F46" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G46" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="H46" s="9">
+      <c r="H46" s="12">
         <v>4</v>
       </c>
-      <c r="I46" s="9" t="s">
+      <c r="I46" s="12" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="47" spans="1:9" ht="15.6">
-      <c r="A47" s="13" t="s">
+      <c r="A47" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B47" s="9">
+      <c r="B47" s="12">
         <v>38</v>
       </c>
-      <c r="C47" s="9" t="s">
+      <c r="C47" s="12" t="s">
         <v>209</v>
       </c>
-      <c r="D47" s="9" t="s">
+      <c r="D47" s="12" t="s">
         <v>210</v>
       </c>
-      <c r="E47" s="9">
+      <c r="E47" s="12">
         <v>2021</v>
       </c>
-      <c r="F47" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="G47" s="9" t="s">
+      <c r="F47" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G47" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="H47" s="9">
+      <c r="H47" s="12">
         <v>2</v>
       </c>
-      <c r="I47" s="9" t="s">
+      <c r="I47" s="12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="48" spans="1:9" ht="15.6">
-      <c r="A48" s="13">
+      <c r="A48" s="12">
         <v>0</v>
       </c>
-      <c r="B48" s="13">
+      <c r="B48" s="12">
         <v>39</v>
       </c>
-      <c r="C48" s="13"/>
-      <c r="D48" s="13"/>
-      <c r="E48" s="13"/>
-      <c r="F48" s="13"/>
-      <c r="G48" s="13"/>
-      <c r="H48" s="13"/>
-      <c r="I48" s="13"/>
+      <c r="C48" s="12"/>
+      <c r="D48" s="12"/>
+      <c r="E48" s="12"/>
+      <c r="F48" s="12"/>
+      <c r="G48" s="12"/>
+      <c r="H48" s="12"/>
+      <c r="I48" s="12"/>
     </row>
     <row r="49" spans="1:9" ht="15.6">
-      <c r="A49" s="13" t="s">
+      <c r="A49" s="12" t="s">
         <v>167</v>
       </c>
-      <c r="B49" s="9">
+      <c r="B49" s="12">
         <v>1</v>
       </c>
-      <c r="C49" s="10" t="s">
+      <c r="C49" s="9" t="s">
         <v>191</v>
       </c>
-      <c r="D49" s="9" t="s">
+      <c r="D49" s="12" t="s">
         <v>192</v>
       </c>
-      <c r="E49" s="9">
+      <c r="E49" s="12">
         <v>1987</v>
       </c>
-      <c r="F49" s="9" t="s">
+      <c r="F49" s="12" t="s">
         <v>217</v>
       </c>
-      <c r="G49" s="9" t="s">
+      <c r="G49" s="12" t="s">
         <v>219</v>
       </c>
-      <c r="H49" s="9">
+      <c r="H49" s="12">
         <v>9</v>
       </c>
-      <c r="I49" s="9" t="s">
+      <c r="I49" s="12" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="50" spans="1:9" ht="15.6">
-      <c r="A50" s="13" t="s">
+      <c r="A50" s="12" t="s">
         <v>167</v>
       </c>
-      <c r="B50" s="9">
+      <c r="B50" s="12">
         <v>2</v>
       </c>
-      <c r="C50" s="9" t="s">
+      <c r="C50" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="D50" s="9" t="s">
+      <c r="D50" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="E50" s="9">
+      <c r="E50" s="12">
         <v>2013</v>
       </c>
-      <c r="F50" s="9" t="s">
+      <c r="F50" s="12" t="s">
         <v>217</v>
       </c>
-      <c r="G50" s="9" t="s">
+      <c r="G50" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="H50" s="9">
+      <c r="H50" s="12">
         <v>7</v>
       </c>
-      <c r="I50" s="9" t="s">
+      <c r="I50" s="12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="51" spans="1:9" ht="15.6">
-      <c r="A51" s="13" t="s">
+      <c r="A51" s="12" t="s">
         <v>167</v>
       </c>
-      <c r="B51" s="9">
+      <c r="B51" s="12">
         <v>3</v>
       </c>
-      <c r="C51" s="9" t="s">
+      <c r="C51" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="D51" s="9" t="s">
+      <c r="D51" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="E51" s="9">
+      <c r="E51" s="12">
         <v>2016</v>
       </c>
-      <c r="F51" s="9" t="s">
+      <c r="F51" s="12" t="s">
         <v>217</v>
       </c>
-      <c r="G51" s="9" t="s">
+      <c r="G51" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="H51" s="9">
+      <c r="H51" s="12">
         <v>3</v>
       </c>
-      <c r="I51" s="9" t="s">
+      <c r="I51" s="12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="52" spans="1:9" ht="15.6">
-      <c r="A52" s="13" t="s">
+      <c r="A52" s="12" t="s">
         <v>167</v>
       </c>
-      <c r="B52" s="9">
+      <c r="B52" s="12">
         <v>4</v>
       </c>
-      <c r="C52" s="9" t="s">
+      <c r="C52" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="D52" s="9" t="s">
+      <c r="D52" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="E52" s="9">
+      <c r="E52" s="12">
         <v>2016</v>
       </c>
-      <c r="F52" s="9" t="s">
+      <c r="F52" s="12" t="s">
         <v>217</v>
       </c>
-      <c r="G52" s="9" t="s">
+      <c r="G52" s="12" t="s">
         <v>219</v>
       </c>
-      <c r="H52" s="9">
+      <c r="H52" s="12">
         <v>2</v>
       </c>
-      <c r="I52" s="9" t="s">
+      <c r="I52" s="12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="53" spans="1:9" ht="15.6">
-      <c r="A53" s="13" t="s">
+      <c r="A53" s="12" t="s">
         <v>167</v>
       </c>
-      <c r="B53" s="9">
+      <c r="B53" s="12">
         <v>5</v>
       </c>
-      <c r="C53" s="9" t="s">
+      <c r="C53" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="D53" s="9" t="s">
+      <c r="D53" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="E53" s="9">
+      <c r="E53" s="12">
         <v>2016</v>
       </c>
-      <c r="F53" s="9" t="s">
+      <c r="F53" s="12" t="s">
         <v>216</v>
       </c>
-      <c r="G53" s="9" t="s">
+      <c r="G53" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="H53" s="9">
+      <c r="H53" s="12">
         <v>6</v>
       </c>
-      <c r="I53" s="9" t="s">
+      <c r="I53" s="12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="54" spans="1:9" ht="15.6">
-      <c r="A54" s="13" t="s">
+      <c r="A54" s="12" t="s">
         <v>167</v>
       </c>
-      <c r="B54" s="9">
+      <c r="B54" s="12">
         <v>6</v>
       </c>
-      <c r="C54" s="9" t="s">
+      <c r="C54" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="D54" s="9" t="s">
+      <c r="D54" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="E54" s="9">
+      <c r="E54" s="12">
         <v>2019</v>
       </c>
-      <c r="F54" s="9" t="s">
+      <c r="F54" s="12" t="s">
         <v>217</v>
       </c>
-      <c r="G54" s="9" t="s">
+      <c r="G54" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="H54" s="9">
+      <c r="H54" s="12">
         <v>2</v>
       </c>
-      <c r="I54" s="9" t="s">
+      <c r="I54" s="12" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="55" spans="1:9" ht="15.6">
-      <c r="A55" s="13" t="s">
+      <c r="A55" s="12" t="s">
         <v>167</v>
       </c>
-      <c r="B55" s="9">
+      <c r="B55" s="12">
         <v>7</v>
       </c>
-      <c r="C55" s="9" t="s">
+      <c r="C55" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="D55" s="9" t="s">
+      <c r="D55" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="E55" s="9">
+      <c r="E55" s="12">
         <v>2019</v>
       </c>
-      <c r="F55" s="9" t="s">
+      <c r="F55" s="12" t="s">
         <v>216</v>
       </c>
-      <c r="G55" s="9" t="s">
+      <c r="G55" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="H55" s="9">
+      <c r="H55" s="12">
         <v>3</v>
       </c>
-      <c r="I55" s="9" t="s">
+      <c r="I55" s="12" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="56" spans="1:9" ht="15.6">
-      <c r="A56" s="13" t="s">
+      <c r="A56" s="12" t="s">
         <v>167</v>
       </c>
-      <c r="B56" s="9">
+      <c r="B56" s="12">
         <v>8</v>
       </c>
-      <c r="C56" s="9" t="s">
+      <c r="C56" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="D56" s="9" t="s">
+      <c r="D56" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="E56" s="9">
+      <c r="E56" s="12">
         <v>2019</v>
       </c>
-      <c r="F56" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="G56" s="9" t="s">
+      <c r="F56" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G56" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="H56" s="9">
+      <c r="H56" s="12">
         <v>4</v>
       </c>
-      <c r="I56" s="9" t="s">
+      <c r="I56" s="12" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="57" spans="1:9" ht="15.6">
-      <c r="A57" s="13" t="s">
+      <c r="A57" s="12" t="s">
         <v>167</v>
       </c>
-      <c r="B57" s="9">
+      <c r="B57" s="12">
         <v>9</v>
       </c>
-      <c r="C57" s="9" t="s">
+      <c r="C57" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="D57" s="9" t="s">
+      <c r="D57" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="E57" s="9">
+      <c r="E57" s="12">
         <v>2019</v>
       </c>
-      <c r="F57" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="G57" s="9" t="s">
+      <c r="F57" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G57" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="H57" s="9">
+      <c r="H57" s="12">
         <v>2</v>
       </c>
-      <c r="I57" s="9" t="s">
+      <c r="I57" s="12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="58" spans="1:9" ht="15.6">
-      <c r="A58" s="13" t="s">
+      <c r="A58" s="12" t="s">
         <v>167</v>
       </c>
-      <c r="B58" s="9">
+      <c r="B58" s="12">
         <v>10</v>
       </c>
-      <c r="C58" s="9" t="s">
+      <c r="C58" s="12" t="s">
         <v>211</v>
       </c>
-      <c r="D58" s="9" t="s">
+      <c r="D58" s="12" t="s">
         <v>212</v>
       </c>
-      <c r="E58" s="9">
+      <c r="E58" s="12">
         <v>2021</v>
       </c>
-      <c r="F58" s="9" t="s">
+      <c r="F58" s="12" t="s">
         <v>217</v>
       </c>
-      <c r="G58" s="9" t="s">
+      <c r="G58" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="H58" s="9">
+      <c r="H58" s="12">
         <v>6</v>
       </c>
-      <c r="I58" s="9" t="s">
+      <c r="I58" s="12" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="59" spans="1:9" ht="15.6">
-      <c r="A59" s="13">
+      <c r="A59" s="12">
         <v>0</v>
       </c>
-      <c r="B59" s="13">
+      <c r="B59" s="12">
         <v>11</v>
       </c>
-      <c r="C59" s="13"/>
-      <c r="D59" s="13"/>
-      <c r="E59" s="13"/>
-      <c r="F59" s="13"/>
-      <c r="G59" s="13"/>
-      <c r="H59" s="13"/>
-      <c r="I59" s="13"/>
+      <c r="C59" s="12"/>
+      <c r="D59" s="12"/>
+      <c r="E59" s="12"/>
+      <c r="F59" s="12"/>
+      <c r="G59" s="12"/>
+      <c r="H59" s="12"/>
+      <c r="I59" s="12"/>
     </row>
     <row r="60" spans="1:9" ht="15.6">
-      <c r="A60" s="13" t="s">
+      <c r="A60" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="B60" s="9">
+      <c r="B60" s="12">
         <v>1</v>
       </c>
-      <c r="C60" s="9" t="s">
+      <c r="C60" s="12" t="s">
         <v>187</v>
       </c>
-      <c r="D60" s="9" t="s">
+      <c r="D60" s="12" t="s">
         <v>188</v>
       </c>
-      <c r="E60" s="9">
+      <c r="E60" s="12">
         <v>1994</v>
       </c>
-      <c r="F60" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="G60" s="9" t="s">
+      <c r="F60" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G60" s="12" t="s">
         <v>219</v>
       </c>
-      <c r="H60" s="9">
+      <c r="H60" s="12">
         <v>3</v>
       </c>
-      <c r="I60" s="9" t="s">
+      <c r="I60" s="12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="61" spans="1:9" ht="15.6">
-      <c r="A61" s="13" t="s">
+      <c r="A61" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="B61" s="9">
+      <c r="B61" s="12">
         <v>2</v>
       </c>
-      <c r="C61" s="10" t="s">
+      <c r="C61" s="9" t="s">
         <v>185</v>
       </c>
-      <c r="D61" s="9" t="s">
+      <c r="D61" s="12" t="s">
         <v>186</v>
       </c>
-      <c r="E61" s="9">
+      <c r="E61" s="12">
         <v>2007</v>
       </c>
-      <c r="F61" s="9" t="s">
+      <c r="F61" s="12" t="s">
         <v>216</v>
       </c>
-      <c r="G61" s="9" t="s">
+      <c r="G61" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="H61" s="9">
+      <c r="H61" s="12">
         <v>10</v>
       </c>
-      <c r="I61" s="9" t="s">
+      <c r="I61" s="12" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="62" spans="1:9" ht="15.6">
-      <c r="A62" s="13" t="s">
+      <c r="A62" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="B62" s="9">
+      <c r="B62" s="12">
         <v>3</v>
       </c>
-      <c r="C62" s="9" t="s">
+      <c r="C62" s="12" t="s">
         <v>221</v>
       </c>
-      <c r="D62" s="9" t="s">
+      <c r="D62" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="E62" s="9">
+      <c r="E62" s="12">
         <v>2011</v>
       </c>
-      <c r="F62" s="9" t="s">
+      <c r="F62" s="12" t="s">
         <v>217</v>
       </c>
-      <c r="G62" s="9" t="s">
+      <c r="G62" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="H62" s="9">
+      <c r="H62" s="12">
         <v>2</v>
       </c>
-      <c r="I62" s="9" t="s">
+      <c r="I62" s="12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="63" spans="1:9" ht="15.6">
-      <c r="A63" s="13" t="s">
+      <c r="A63" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="B63" s="9">
+      <c r="B63" s="12">
         <v>4</v>
       </c>
-      <c r="C63" s="9" t="s">
+      <c r="C63" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="D63" s="9" t="s">
+      <c r="D63" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="E63" s="9">
+      <c r="E63" s="12">
         <v>2011</v>
       </c>
-      <c r="F63" s="9" t="s">
+      <c r="F63" s="12" t="s">
         <v>217</v>
       </c>
-      <c r="G63" s="9" t="s">
+      <c r="G63" s="12" t="s">
         <v>219</v>
       </c>
-      <c r="H63" s="9">
+      <c r="H63" s="12">
         <v>10</v>
       </c>
-      <c r="I63" s="9" t="s">
+      <c r="I63" s="12" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="64" spans="1:9" ht="15.6">
-      <c r="A64" s="13" t="s">
+      <c r="A64" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="B64" s="9">
+      <c r="B64" s="12">
         <v>5</v>
       </c>
-      <c r="C64" s="9" t="s">
+      <c r="C64" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="D64" s="9" t="s">
+      <c r="D64" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="E64" s="9">
+      <c r="E64" s="12">
         <v>2019</v>
       </c>
-      <c r="F64" s="9" t="s">
+      <c r="F64" s="12" t="s">
         <v>217</v>
       </c>
-      <c r="G64" s="9" t="s">
+      <c r="G64" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="H64" s="9">
+      <c r="H64" s="12">
         <v>2</v>
       </c>
-      <c r="I64" s="9" t="s">
+      <c r="I64" s="12" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="65" spans="1:9" ht="15.6">
-      <c r="A65" s="13" t="s">
+      <c r="A65" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="B65" s="9">
+      <c r="B65" s="12">
         <v>6</v>
       </c>
-      <c r="C65" s="9" t="s">
+      <c r="C65" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="D65" s="9" t="s">
+      <c r="D65" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="E65" s="9">
+      <c r="E65" s="12">
         <v>2019</v>
       </c>
-      <c r="F65" s="9" t="s">
+      <c r="F65" s="12" t="s">
         <v>217</v>
       </c>
-      <c r="G65" s="9" t="s">
+      <c r="G65" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="H65" s="9">
+      <c r="H65" s="12">
         <v>4</v>
       </c>
-      <c r="I65" s="9" t="s">
+      <c r="I65" s="12" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="66" spans="1:9" ht="15.6">
-      <c r="A66" s="13" t="s">
+      <c r="A66" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="B66" s="9">
+      <c r="B66" s="12">
         <v>7</v>
       </c>
-      <c r="C66" s="9" t="s">
+      <c r="C66" s="12" t="s">
         <v>120</v>
       </c>
-      <c r="D66" s="9" t="s">
+      <c r="D66" s="12" t="s">
         <v>222</v>
       </c>
-      <c r="E66" s="9">
+      <c r="E66" s="12">
         <v>2019</v>
       </c>
-      <c r="F66" s="9" t="s">
+      <c r="F66" s="12" t="s">
         <v>216</v>
       </c>
-      <c r="G66" s="9" t="s">
+      <c r="G66" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="H66" s="9">
+      <c r="H66" s="12">
         <v>2</v>
       </c>
-      <c r="I66" s="9" t="s">
+      <c r="I66" s="12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="67" spans="1:9" ht="15.6">
-      <c r="A67" s="13" t="s">
+      <c r="A67" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="B67" s="9">
+      <c r="B67" s="12">
         <v>8</v>
       </c>
-      <c r="C67" s="9" t="s">
+      <c r="C67" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="D67" s="9" t="s">
+      <c r="D67" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="E67" s="9">
+      <c r="E67" s="12">
         <v>2019</v>
       </c>
-      <c r="F67" s="9" t="s">
+      <c r="F67" s="12" t="s">
         <v>216</v>
       </c>
-      <c r="G67" s="9" t="s">
+      <c r="G67" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="H67" s="9">
+      <c r="H67" s="12">
         <v>2</v>
       </c>
-      <c r="I67" s="9" t="s">
+      <c r="I67" s="12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="68" spans="1:9" ht="15.6">
-      <c r="A68" s="13" t="s">
+      <c r="A68" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="B68" s="9">
+      <c r="B68" s="12">
         <v>9</v>
       </c>
-      <c r="C68" s="9" t="s">
+      <c r="C68" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="D68" s="9" t="s">
+      <c r="D68" s="12" t="s">
         <v>125</v>
       </c>
-      <c r="E68" s="9">
+      <c r="E68" s="12">
         <v>2019</v>
       </c>
-      <c r="F68" s="9" t="s">
+      <c r="F68" s="12" t="s">
         <v>216</v>
       </c>
-      <c r="G68" s="9" t="s">
+      <c r="G68" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="H68" s="9">
+      <c r="H68" s="12">
         <v>6</v>
       </c>
-      <c r="I68" s="9" t="s">
+      <c r="I68" s="12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="69" spans="1:9" ht="15.6">
-      <c r="A69" s="13" t="s">
+      <c r="A69" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="B69" s="9">
+      <c r="B69" s="12">
         <v>10</v>
       </c>
-      <c r="C69" s="9" t="s">
+      <c r="C69" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="D69" s="9" t="s">
+      <c r="D69" s="12" t="s">
         <v>127</v>
       </c>
-      <c r="E69" s="9">
+      <c r="E69" s="12">
         <v>2020</v>
       </c>
-      <c r="F69" s="9" t="s">
+      <c r="F69" s="12" t="s">
         <v>216</v>
       </c>
-      <c r="G69" s="9" t="s">
+      <c r="G69" s="12" t="s">
         <v>219</v>
       </c>
-      <c r="H69" s="9">
+      <c r="H69" s="12">
         <v>4</v>
       </c>
-      <c r="I69" s="9" t="s">
+      <c r="I69" s="12" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="70" spans="1:9" ht="15.6">
-      <c r="A70" s="13" t="s">
+      <c r="A70" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="B70" s="9">
+      <c r="B70" s="12">
         <v>11</v>
       </c>
-      <c r="C70" s="11" t="s">
+      <c r="C70" s="10" t="s">
         <v>172</v>
       </c>
-      <c r="D70" s="9" t="s">
+      <c r="D70" s="12" t="s">
         <v>173</v>
       </c>
-      <c r="E70" s="9">
+      <c r="E70" s="12">
         <v>2020</v>
       </c>
-      <c r="F70" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="G70" s="9" t="s">
+      <c r="F70" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G70" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="H70" s="9">
+      <c r="H70" s="12">
         <v>2</v>
       </c>
-      <c r="I70" s="9" t="s">
+      <c r="I70" s="12" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="71" spans="1:9" ht="15.6">
-      <c r="A71" s="13" t="s">
+      <c r="A71" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="B71" s="9">
+      <c r="B71" s="12">
         <v>12</v>
       </c>
-      <c r="C71" s="10" t="s">
+      <c r="C71" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="D71" s="9" t="s">
+      <c r="D71" s="12" t="s">
         <v>180</v>
       </c>
-      <c r="E71" s="9">
+      <c r="E71" s="12">
         <v>2020</v>
       </c>
-      <c r="F71" s="9" t="s">
+      <c r="F71" s="12" t="s">
         <v>217</v>
       </c>
-      <c r="G71" s="9" t="s">
+      <c r="G71" s="12" t="s">
         <v>219</v>
       </c>
-      <c r="H71" s="9">
+      <c r="H71" s="12">
         <v>2</v>
       </c>
-      <c r="I71" s="9" t="s">
+      <c r="I71" s="12" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="72" spans="1:9" ht="15.6">
-      <c r="A72" s="13">
+      <c r="A72" s="12">
         <v>0</v>
       </c>
-      <c r="B72" s="13">
-        <v>13</v>
-      </c>
-      <c r="C72" s="10"/>
-      <c r="D72" s="13"/>
-      <c r="E72" s="13"/>
-      <c r="F72" s="13"/>
-      <c r="G72" s="13"/>
-      <c r="H72" s="13"/>
-      <c r="I72" s="13"/>
+      <c r="B72" s="12">
+        <v>13</v>
+      </c>
+      <c r="C72" s="9"/>
+      <c r="D72" s="12"/>
+      <c r="E72" s="12"/>
+      <c r="F72" s="12"/>
+      <c r="G72" s="12"/>
+      <c r="H72" s="12"/>
+      <c r="I72" s="12"/>
     </row>
     <row r="73" spans="1:9" ht="15.6">
-      <c r="A73" s="13" t="s">
+      <c r="A73" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="B73" s="9">
+      <c r="B73" s="12">
         <v>1</v>
       </c>
-      <c r="C73" s="9" t="s">
+      <c r="C73" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="D73" s="9" t="s">
+      <c r="D73" s="12" t="s">
         <v>130</v>
       </c>
-      <c r="E73" s="9">
+      <c r="E73" s="12">
         <v>2006</v>
       </c>
-      <c r="F73" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="G73" s="9" t="s">
+      <c r="F73" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G73" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="H73" s="9">
+      <c r="H73" s="12">
         <v>5</v>
       </c>
-      <c r="I73" s="9" t="s">
+      <c r="I73" s="12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="74" spans="1:9" ht="15.6">
-      <c r="A74" s="13" t="s">
+      <c r="A74" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="B74" s="9">
+      <c r="B74" s="12">
         <v>2</v>
       </c>
-      <c r="C74" s="9" t="s">
+      <c r="C74" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="D74" s="9" t="s">
+      <c r="D74" s="12" t="s">
         <v>132</v>
       </c>
-      <c r="E74" s="9">
+      <c r="E74" s="12">
         <v>2008</v>
       </c>
-      <c r="F74" s="9" t="s">
+      <c r="F74" s="12" t="s">
         <v>217</v>
       </c>
-      <c r="G74" s="9" t="s">
+      <c r="G74" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="H74" s="9">
+      <c r="H74" s="12">
         <v>4</v>
       </c>
-      <c r="I74" s="9" t="s">
+      <c r="I74" s="12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="75" spans="1:9" ht="15.6">
-      <c r="A75" s="13" t="s">
+      <c r="A75" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="B75" s="9">
+      <c r="B75" s="12">
         <v>3</v>
       </c>
-      <c r="C75" s="9" t="s">
+      <c r="C75" s="12" t="s">
         <v>135</v>
       </c>
-      <c r="D75" s="9" t="s">
+      <c r="D75" s="12" t="s">
         <v>136</v>
       </c>
-      <c r="E75" s="9">
+      <c r="E75" s="12">
         <v>2016</v>
       </c>
-      <c r="F75" s="9" t="s">
+      <c r="F75" s="12" t="s">
         <v>216</v>
       </c>
-      <c r="G75" s="9" t="s">
+      <c r="G75" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="H75" s="9">
+      <c r="H75" s="12">
         <v>4</v>
       </c>
-      <c r="I75" s="9" t="s">
+      <c r="I75" s="12" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="76" spans="1:9" ht="15.6">
-      <c r="A76" s="13" t="s">
+      <c r="A76" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="B76" s="9">
+      <c r="B76" s="12">
         <v>4</v>
       </c>
-      <c r="C76" s="9" t="s">
+      <c r="C76" s="12" t="s">
         <v>137</v>
       </c>
-      <c r="D76" s="9" t="s">
+      <c r="D76" s="12" t="s">
         <v>138</v>
       </c>
-      <c r="E76" s="9">
+      <c r="E76" s="12">
         <v>2017</v>
       </c>
-      <c r="F76" s="9" t="s">
+      <c r="F76" s="12" t="s">
         <v>217</v>
       </c>
-      <c r="G76" s="9" t="s">
+      <c r="G76" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="H76" s="9">
+      <c r="H76" s="12">
         <v>5</v>
       </c>
-      <c r="I76" s="9" t="s">
+      <c r="I76" s="12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="77" spans="1:9" ht="15.6">
-      <c r="A77" s="13" t="s">
+      <c r="A77" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="B77" s="9">
+      <c r="B77" s="12">
         <v>5</v>
       </c>
-      <c r="C77" s="9" t="s">
+      <c r="C77" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="D77" s="9" t="s">
+      <c r="D77" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="E77" s="9">
+      <c r="E77" s="12">
         <v>2018</v>
       </c>
-      <c r="F77" s="9" t="s">
+      <c r="F77" s="12" t="s">
         <v>217</v>
       </c>
-      <c r="G77" s="9" t="s">
+      <c r="G77" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="H77" s="9">
+      <c r="H77" s="12">
         <v>8</v>
       </c>
-      <c r="I77" s="9" t="s">
+      <c r="I77" s="12" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="78" spans="1:9" ht="15.6">
-      <c r="A78" s="13" t="s">
+      <c r="A78" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="B78" s="9">
+      <c r="B78" s="12">
         <v>6</v>
       </c>
-      <c r="C78" s="9" t="s">
+      <c r="C78" s="12" t="s">
         <v>139</v>
       </c>
-      <c r="D78" s="9" t="s">
+      <c r="D78" s="12" t="s">
         <v>140</v>
       </c>
-      <c r="E78" s="9">
+      <c r="E78" s="12">
         <v>2019</v>
       </c>
-      <c r="F78" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="G78" s="9" t="s">
+      <c r="F78" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G78" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="H78" s="9">
+      <c r="H78" s="12">
         <v>12</v>
       </c>
-      <c r="I78" s="9" t="s">
+      <c r="I78" s="12" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="79" spans="1:9" ht="15.6">
-      <c r="A79" s="13" t="s">
+      <c r="A79" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="B79" s="9">
+      <c r="B79" s="12">
         <v>7</v>
       </c>
-      <c r="C79" s="9" t="s">
+      <c r="C79" s="12" t="s">
         <v>157</v>
       </c>
-      <c r="D79" s="9" t="s">
+      <c r="D79" s="12" t="s">
         <v>158</v>
       </c>
-      <c r="E79" s="9">
+      <c r="E79" s="12">
         <v>2020</v>
       </c>
-      <c r="F79" s="9" t="s">
+      <c r="F79" s="12" t="s">
         <v>217</v>
       </c>
-      <c r="G79" s="9" t="s">
+      <c r="G79" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="H79" s="9">
+      <c r="H79" s="12">
         <v>3</v>
       </c>
-      <c r="I79" s="9" t="s">
+      <c r="I79" s="12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="80" spans="1:9" ht="15.6">
-      <c r="A80" s="13">
+      <c r="A80" s="12">
         <v>0</v>
       </c>
-      <c r="B80" s="13">
+      <c r="B80" s="12">
         <v>8</v>
       </c>
-      <c r="C80" s="13"/>
-      <c r="D80" s="13"/>
-      <c r="E80" s="13"/>
-      <c r="F80" s="13"/>
-      <c r="G80" s="13"/>
-      <c r="H80" s="13"/>
-      <c r="I80" s="13"/>
+      <c r="C80" s="12"/>
+      <c r="D80" s="12"/>
+      <c r="E80" s="12"/>
+      <c r="F80" s="12"/>
+      <c r="G80" s="12"/>
+      <c r="H80" s="12"/>
+      <c r="I80" s="12"/>
     </row>
     <row r="81" spans="1:9" ht="15.6">
-      <c r="A81" s="13" t="s">
+      <c r="A81" s="12" t="s">
         <v>143</v>
       </c>
-      <c r="B81" s="9">
+      <c r="B81" s="12">
         <v>1</v>
       </c>
-      <c r="C81" s="9" t="s">
+      <c r="C81" s="12" t="s">
         <v>144</v>
       </c>
-      <c r="D81" s="9" t="s">
+      <c r="D81" s="12" t="s">
         <v>145</v>
       </c>
-      <c r="E81" s="9">
+      <c r="E81" s="12">
         <v>2018</v>
       </c>
-      <c r="F81" s="9" t="s">
+      <c r="F81" s="12" t="s">
         <v>217</v>
       </c>
-      <c r="G81" s="9" t="s">
+      <c r="G81" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="H81" s="9">
+      <c r="H81" s="12">
         <v>4</v>
       </c>
-      <c r="I81" s="9" t="s">
+      <c r="I81" s="12" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="82" spans="1:9" ht="15.6">
-      <c r="A82" s="13" t="s">
+      <c r="A82" s="12" t="s">
         <v>143</v>
       </c>
-      <c r="B82" s="9">
+      <c r="B82" s="12">
         <v>2</v>
       </c>
-      <c r="C82" s="10" t="s">
+      <c r="C82" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="D82" s="9" t="s">
+      <c r="D82" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="E82" s="9">
+      <c r="E82" s="12">
         <v>2012</v>
       </c>
-      <c r="F82" s="9" t="s">
+      <c r="F82" s="12" t="s">
         <v>217</v>
       </c>
-      <c r="G82" s="9" t="s">
+      <c r="G82" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="H82" s="9">
+      <c r="H82" s="12">
         <v>5</v>
       </c>
-      <c r="I82" s="9" t="s">
+      <c r="I82" s="12" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="83" spans="1:9" ht="15.6">
-      <c r="A83" s="13" t="s">
+      <c r="A83" s="12" t="s">
         <v>143</v>
       </c>
-      <c r="B83" s="9">
+      <c r="B83" s="12">
         <v>3</v>
       </c>
-      <c r="C83" s="9" t="s">
+      <c r="C83" s="12" t="s">
         <v>146</v>
       </c>
-      <c r="D83" s="9" t="s">
+      <c r="D83" s="12" t="s">
         <v>147</v>
       </c>
-      <c r="E83" s="9">
+      <c r="E83" s="12">
         <v>2019</v>
       </c>
-      <c r="F83" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="G83" s="9" t="s">
+      <c r="F83" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G83" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="H83" s="9">
+      <c r="H83" s="12">
         <v>2</v>
       </c>
-      <c r="I83" s="9" t="s">
+      <c r="I83" s="12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="84" spans="1:9" ht="15.6">
-      <c r="A84" s="13">
+      <c r="A84" s="12">
         <v>0</v>
       </c>
-      <c r="B84" s="13">
+      <c r="B84" s="12">
         <v>4</v>
       </c>
-      <c r="C84" s="13"/>
-      <c r="D84" s="13"/>
-      <c r="E84" s="13"/>
-      <c r="F84" s="13"/>
-      <c r="G84" s="13"/>
-      <c r="H84" s="13"/>
-      <c r="I84" s="13"/>
+      <c r="C84" s="12"/>
+      <c r="D84" s="12"/>
+      <c r="E84" s="12"/>
+      <c r="F84" s="12"/>
+      <c r="G84" s="12"/>
+      <c r="H84" s="12"/>
+      <c r="I84" s="12"/>
     </row>
     <row r="85" spans="1:9" ht="15.6">
-      <c r="A85" s="13" t="s">
+      <c r="A85" s="12" t="s">
         <v>148</v>
       </c>
-      <c r="B85" s="9">
+      <c r="B85" s="12">
         <v>1</v>
       </c>
-      <c r="C85" s="10" t="s">
+      <c r="C85" s="9" t="s">
         <v>189</v>
       </c>
-      <c r="D85" s="9" t="s">
+      <c r="D85" s="12" t="s">
         <v>190</v>
       </c>
-      <c r="E85" s="9">
+      <c r="E85" s="12">
         <v>1993</v>
       </c>
-      <c r="F85" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="G85" s="9" t="s">
+      <c r="F85" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G85" s="12" t="s">
         <v>219</v>
       </c>
-      <c r="H85" s="9">
+      <c r="H85" s="12">
         <v>3</v>
       </c>
-      <c r="I85" s="9" t="s">
+      <c r="I85" s="12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="86" spans="1:9" ht="15.6">
-      <c r="A86" s="13" t="s">
+      <c r="A86" s="12" t="s">
         <v>148</v>
       </c>
-      <c r="B86" s="9">
+      <c r="B86" s="12">
         <v>2</v>
       </c>
-      <c r="C86" s="9" t="s">
+      <c r="C86" s="12" t="s">
         <v>149</v>
       </c>
-      <c r="D86" s="9" t="s">
+      <c r="D86" s="12" t="s">
         <v>150</v>
       </c>
-      <c r="E86" s="9">
+      <c r="E86" s="12">
         <v>2016</v>
       </c>
-      <c r="F86" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="G86" s="9" t="s">
+      <c r="F86" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G86" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="H86" s="9">
+      <c r="H86" s="12">
         <v>2</v>
       </c>
-      <c r="I86" s="9" t="s">
+      <c r="I86" s="12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="87" spans="1:9" ht="15.6">
-      <c r="A87" s="13" t="s">
+      <c r="A87" s="12" t="s">
         <v>148</v>
       </c>
-      <c r="B87" s="9">
+      <c r="B87" s="12">
         <v>3</v>
       </c>
-      <c r="C87" s="10" t="s">
+      <c r="C87" s="12" t="s">
+        <v>226</v>
+      </c>
+      <c r="D87" s="12" t="s">
+        <v>227</v>
+      </c>
+      <c r="E87" s="12">
+        <v>2020</v>
+      </c>
+      <c r="F87" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G87" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="H87" s="12">
+        <v>3</v>
+      </c>
+      <c r="I87" s="12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" ht="15.6">
+      <c r="A88" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="B88" s="12">
+        <v>4</v>
+      </c>
+      <c r="C88" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="D87" s="9" t="s">
+      <c r="D88" s="12" t="s">
         <v>208</v>
       </c>
-      <c r="E87" s="9">
+      <c r="E88" s="12">
         <v>2021</v>
       </c>
-      <c r="F87" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="G87" s="9" t="s">
+      <c r="F88" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G88" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="H87" s="9">
+      <c r="H88" s="12">
         <v>6</v>
       </c>
-      <c r="I87" s="9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="88" spans="1:9" ht="15.6">
-      <c r="A88" s="13">
+      <c r="I88" s="12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" ht="15.6">
+      <c r="A89" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="B89" s="12">
+        <v>5</v>
+      </c>
+      <c r="C89" s="14" t="s">
+        <v>228</v>
+      </c>
+      <c r="D89" s="14" t="s">
+        <v>229</v>
+      </c>
+      <c r="E89" s="14">
+        <v>2021</v>
+      </c>
+      <c r="F89" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G89" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="H89" s="14">
+        <v>2</v>
+      </c>
+      <c r="I89" s="14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9">
+      <c r="A90" s="14">
         <v>0</v>
       </c>
-      <c r="B88" s="13">
+      <c r="B90" s="14">
+        <v>6</v>
+      </c>
+      <c r="C90" s="14"/>
+      <c r="D90" s="14"/>
+      <c r="E90" s="14"/>
+      <c r="F90" s="14"/>
+      <c r="G90" s="14"/>
+      <c r="H90" s="14"/>
+      <c r="I90" s="14"/>
+    </row>
+    <row r="91" spans="1:9" ht="15.6">
+      <c r="A91" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="B91" s="12">
+        <v>1</v>
+      </c>
+      <c r="C91" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="D91" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="E91" s="12">
+        <v>2001</v>
+      </c>
+      <c r="F91" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G91" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="H91" s="12">
+        <v>5</v>
+      </c>
+      <c r="I91" s="12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" ht="15.6">
+      <c r="A92" s="12">
+        <v>0</v>
+      </c>
+      <c r="B92" s="12">
+        <v>2</v>
+      </c>
+      <c r="C92" s="12"/>
+      <c r="D92" s="12"/>
+      <c r="E92" s="12"/>
+      <c r="F92" s="12"/>
+      <c r="G92" s="12"/>
+      <c r="H92" s="12"/>
+      <c r="I92" s="12"/>
+    </row>
+    <row r="93" spans="1:9" ht="15.6">
+      <c r="A93" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="B93" s="12">
+        <v>1</v>
+      </c>
+      <c r="C93" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="D93" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="E93" s="12">
+        <v>1997</v>
+      </c>
+      <c r="F93" s="12" t="s">
+        <v>217</v>
+      </c>
+      <c r="G93" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="H93" s="12">
         <v>4</v>
       </c>
-      <c r="C88" s="10"/>
-      <c r="D88" s="13"/>
-      <c r="E88" s="13"/>
-      <c r="F88" s="13"/>
-      <c r="G88" s="13"/>
-      <c r="H88" s="13"/>
-      <c r="I88" s="13"/>
-    </row>
-    <row r="89" spans="1:9" ht="15.6">
-      <c r="A89" s="13" t="s">
-        <v>151</v>
-      </c>
-      <c r="B89" s="9">
+      <c r="I93" s="12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" ht="15.6">
+      <c r="A94" s="12">
+        <v>0</v>
+      </c>
+      <c r="B94" s="12">
+        <v>2</v>
+      </c>
+      <c r="C94" s="11"/>
+      <c r="D94" s="12"/>
+      <c r="E94" s="12"/>
+      <c r="F94" s="12"/>
+      <c r="G94" s="12"/>
+      <c r="H94" s="12"/>
+      <c r="I94" s="12"/>
+    </row>
+    <row r="95" spans="1:9" ht="15.6" customHeight="1">
+      <c r="A95" s="12" t="s">
+        <v>225</v>
+      </c>
+      <c r="B95" s="12">
         <v>1</v>
       </c>
-      <c r="C89" s="9" t="s">
-        <v>152</v>
-      </c>
-      <c r="D89" s="9" t="s">
-        <v>153</v>
-      </c>
-      <c r="E89" s="9">
-        <v>2001</v>
-      </c>
-      <c r="F89" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="G89" s="9" t="s">
+      <c r="C95" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="D95" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="E95" s="12">
+        <v>2014</v>
+      </c>
+      <c r="F95" s="12"/>
+      <c r="G95" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="H89" s="9">
+      <c r="H95" s="12">
+        <v>2</v>
+      </c>
+      <c r="I95" s="12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" ht="15.6">
+      <c r="A96" s="12" t="s">
+        <v>225</v>
+      </c>
+      <c r="B96" s="12">
+        <v>2</v>
+      </c>
+      <c r="C96" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="D96" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="E96" s="12">
+        <v>2015</v>
+      </c>
+      <c r="F96" s="12"/>
+      <c r="G96" s="12" t="s">
+        <v>219</v>
+      </c>
+      <c r="H96" s="12">
         <v>5</v>
       </c>
-      <c r="I89" s="9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="90" spans="1:9" ht="15.6">
-      <c r="A90" s="13">
-        <v>0</v>
-      </c>
-      <c r="B90" s="13">
+      <c r="I96" s="12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" ht="15.6">
+      <c r="A97" s="12" t="s">
+        <v>225</v>
+      </c>
+      <c r="B97" s="12">
+        <v>3</v>
+      </c>
+      <c r="C97" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="D97" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="E97" s="12">
+        <v>2018</v>
+      </c>
+      <c r="F97" s="12"/>
+      <c r="G97" s="12" t="s">
+        <v>219</v>
+      </c>
+      <c r="H97" s="12">
+        <v>6</v>
+      </c>
+      <c r="I97" s="12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" ht="15.6">
+      <c r="A98" s="12" t="s">
+        <v>225</v>
+      </c>
+      <c r="B98" s="12">
+        <v>4</v>
+      </c>
+      <c r="C98" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="D98" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="E98" s="12">
+        <v>2018</v>
+      </c>
+      <c r="F98" s="12"/>
+      <c r="G98" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="H98" s="12">
         <v>2</v>
       </c>
-      <c r="C90" s="13"/>
-      <c r="D90" s="13"/>
-      <c r="E90" s="13"/>
-      <c r="F90" s="13"/>
-      <c r="G90" s="13"/>
-      <c r="H90" s="13"/>
-      <c r="I90" s="13"/>
-    </row>
-    <row r="91" spans="1:9" ht="15.6">
-      <c r="A91" s="13" t="s">
-        <v>166</v>
-      </c>
-      <c r="B91" s="9">
-        <v>1</v>
-      </c>
-      <c r="C91" s="12" t="s">
-        <v>154</v>
-      </c>
-      <c r="D91" s="9" t="s">
-        <v>155</v>
-      </c>
-      <c r="E91" s="9">
-        <v>1997</v>
-      </c>
-      <c r="F91" s="9" t="s">
-        <v>217</v>
-      </c>
-      <c r="G91" s="9" t="s">
+      <c r="I98" s="12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" ht="15.6">
+      <c r="A99" s="12" t="s">
+        <v>225</v>
+      </c>
+      <c r="B99" s="12">
+        <v>5</v>
+      </c>
+      <c r="C99" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="D99" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="E99" s="12">
+        <v>2019</v>
+      </c>
+      <c r="F99" s="12"/>
+      <c r="G99" s="12" t="s">
+        <v>219</v>
+      </c>
+      <c r="H99" s="12">
+        <v>6</v>
+      </c>
+      <c r="I99" s="12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" ht="15.6">
+      <c r="A100" s="12" t="s">
+        <v>225</v>
+      </c>
+      <c r="B100" s="12">
+        <v>6</v>
+      </c>
+      <c r="C100" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="D100" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="E100" s="12">
+        <v>2019</v>
+      </c>
+      <c r="F100" s="12"/>
+      <c r="G100" s="12" t="s">
+        <v>219</v>
+      </c>
+      <c r="H100" s="12">
+        <v>3</v>
+      </c>
+      <c r="I100" s="12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" ht="15.6">
+      <c r="A101" s="12" t="s">
+        <v>225</v>
+      </c>
+      <c r="B101" s="12">
+        <v>7</v>
+      </c>
+      <c r="C101" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="D101" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="E101" s="12">
+        <v>2020</v>
+      </c>
+      <c r="F101" s="12"/>
+      <c r="G101" s="12" t="s">
+        <v>219</v>
+      </c>
+      <c r="H101" s="12">
+        <v>2</v>
+      </c>
+      <c r="I101" s="12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" ht="15.6">
+      <c r="A102" s="12" t="s">
+        <v>225</v>
+      </c>
+      <c r="B102" s="12">
+        <v>8</v>
+      </c>
+      <c r="C102" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="D102" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="E102" s="12">
+        <v>2020</v>
+      </c>
+      <c r="F102" s="12"/>
+      <c r="G102" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="H91" s="9">
-        <v>4</v>
-      </c>
-      <c r="I91" s="9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="92" spans="1:9" ht="15.6">
-      <c r="A92" s="13">
-        <v>0</v>
-      </c>
-      <c r="B92" s="13">
-        <v>2</v>
-      </c>
-      <c r="C92" s="12"/>
-      <c r="D92" s="13"/>
-      <c r="E92" s="13"/>
-      <c r="F92" s="13"/>
-      <c r="G92" s="13"/>
-      <c r="H92" s="13"/>
-      <c r="I92" s="13"/>
-    </row>
-    <row r="93" spans="1:9" ht="15.6" customHeight="1">
-      <c r="A93" s="13" t="s">
-        <v>225</v>
-      </c>
-      <c r="B93" s="9">
-        <v>1</v>
-      </c>
-      <c r="C93" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="D93" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="E93" s="9">
-        <v>2014</v>
-      </c>
-      <c r="F93" s="9"/>
-      <c r="G93" s="9" t="s">
-        <v>220</v>
-      </c>
-      <c r="H93" s="9">
-        <v>2</v>
-      </c>
-      <c r="I93" s="9" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="94" spans="1:9" ht="15.6">
-      <c r="A94" s="13" t="s">
-        <v>225</v>
-      </c>
-      <c r="B94" s="9">
-        <v>2</v>
-      </c>
-      <c r="C94" s="9" t="s">
-        <v>133</v>
-      </c>
-      <c r="D94" s="9" t="s">
-        <v>134</v>
-      </c>
-      <c r="E94" s="9">
-        <v>2015</v>
-      </c>
-      <c r="F94" s="9"/>
-      <c r="G94" s="9" t="s">
-        <v>219</v>
-      </c>
-      <c r="H94" s="9">
+      <c r="H102" s="12">
         <v>5</v>
       </c>
-      <c r="I94" s="9" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="95" spans="1:9" ht="15.6">
-      <c r="A95" s="13" t="s">
-        <v>225</v>
-      </c>
-      <c r="B95" s="9">
-        <v>3</v>
-      </c>
-      <c r="C95" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="D95" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="E95" s="9">
-        <v>2018</v>
-      </c>
-      <c r="F95" s="9"/>
-      <c r="G95" s="9" t="s">
-        <v>219</v>
-      </c>
-      <c r="H95" s="9">
-        <v>6</v>
-      </c>
-      <c r="I95" s="9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="96" spans="1:9" ht="15.6">
-      <c r="A96" s="13" t="s">
-        <v>225</v>
-      </c>
-      <c r="B96" s="9">
-        <v>4</v>
-      </c>
-      <c r="C96" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="D96" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="E96" s="9">
-        <v>2018</v>
-      </c>
-      <c r="F96" s="9"/>
-      <c r="G96" s="9" t="s">
-        <v>220</v>
-      </c>
-      <c r="H96" s="9">
-        <v>2</v>
-      </c>
-      <c r="I96" s="9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="97" spans="1:9" ht="15.6">
-      <c r="A97" s="13" t="s">
-        <v>225</v>
-      </c>
-      <c r="B97" s="9">
-        <v>5</v>
-      </c>
-      <c r="C97" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="D97" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="E97" s="9">
-        <v>2019</v>
-      </c>
-      <c r="F97" s="9"/>
-      <c r="G97" s="9" t="s">
-        <v>219</v>
-      </c>
-      <c r="H97" s="9">
-        <v>6</v>
-      </c>
-      <c r="I97" s="9" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="98" spans="1:9" ht="15.6">
-      <c r="A98" s="13" t="s">
-        <v>225</v>
-      </c>
-      <c r="B98" s="9">
-        <v>6</v>
-      </c>
-      <c r="C98" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="D98" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="E98" s="9">
-        <v>2019</v>
-      </c>
-      <c r="F98" s="9"/>
-      <c r="G98" s="9" t="s">
-        <v>219</v>
-      </c>
-      <c r="H98" s="9">
-        <v>3</v>
-      </c>
-      <c r="I98" s="9" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="99" spans="1:9" ht="15.6">
-      <c r="A99" s="13" t="s">
-        <v>225</v>
-      </c>
-      <c r="B99" s="9">
-        <v>7</v>
-      </c>
-      <c r="C99" s="12" t="s">
-        <v>161</v>
-      </c>
-      <c r="D99" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="E99" s="9">
-        <v>2020</v>
-      </c>
-      <c r="F99" s="9"/>
-      <c r="G99" s="9" t="s">
-        <v>219</v>
-      </c>
-      <c r="H99" s="9">
-        <v>2</v>
-      </c>
-      <c r="I99" s="9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="100" spans="1:9" ht="15.6">
-      <c r="A100" s="13" t="s">
-        <v>225</v>
-      </c>
-      <c r="B100" s="9">
-        <v>8</v>
-      </c>
-      <c r="C100" s="9" t="s">
-        <v>141</v>
-      </c>
-      <c r="D100" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="E100" s="9">
-        <v>2020</v>
-      </c>
-      <c r="F100" s="9"/>
-      <c r="G100" s="9" t="s">
-        <v>220</v>
-      </c>
-      <c r="H100" s="9">
-        <v>5</v>
-      </c>
-      <c r="I100" s="9" t="s">
+      <c r="I102" s="12" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>